<commit_message>
some changes to report
added BOM and code
</commit_message>
<xml_diff>
--- a/Documentation/BillOfMaterials_rev2.xlsx
+++ b/Documentation/BillOfMaterials_rev2.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="435" windowWidth="20835" windowHeight="9765"/>
   </bookViews>
   <sheets>
-    <sheet name="MSGP_BOM" sheetId="3" r:id="rId1"/>
-    <sheet name="ISI_BOM" sheetId="1" r:id="rId2"/>
+    <sheet name="ISI_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="MSGP_BOM" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -973,68 +973,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1529073" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2305050" y="428625"/>
-          <a:ext cx="1529073" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>MSGPCost</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> Breakdown </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1139,6 +1077,68 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
             <a:t>  Cost Breakdowm </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1529073" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2305050" y="428625"/>
+          <a:ext cx="1529073" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>MSGPCost</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> Breakdown </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
@@ -1436,315 +1436,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G21"/>
+  <dimension ref="A4:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="G6" s="14">
-        <f t="shared" ref="G6:G14" si="0">F6*A6</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>19</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="G7" s="14">
-        <f t="shared" si="0"/>
-        <v>1.9000000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="11">
-        <v>1.76</v>
-      </c>
-      <c r="G8" s="14">
-        <f t="shared" si="0"/>
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G9" s="14">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G10" s="14">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G11" s="14">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>3</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G12" s="14">
-        <f t="shared" si="0"/>
-        <v>1.6800000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="11">
-        <v>3.32</v>
-      </c>
-      <c r="G13" s="14">
-        <f t="shared" si="0"/>
-        <v>3.32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0.88</v>
-      </c>
-      <c r="G14" s="14">
-        <f t="shared" si="0"/>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="15">
-        <f>SUM(G6:G14)</f>
-        <v>12.540000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="10">
-        <f>SUM(G16,G19)</f>
-        <v>12.540000000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -2398,4 +2092,310 @@
   <pageSetup paperSize="0" orientation="landscape" r:id="rId8"/>
   <drawing r:id="rId9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" ref="G6:G14" si="0">F6*A6</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1.76</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="0"/>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G12" s="14">
+        <f t="shared" si="0"/>
+        <v>1.6800000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="11">
+        <v>3.32</v>
+      </c>
+      <c r="G13" s="14">
+        <f t="shared" si="0"/>
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="G14" s="14">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="15">
+        <f>SUM(G6:G14)</f>
+        <v>12.540000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="10">
+        <f>SUM(G16,G19)</f>
+        <v>12.540000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>